<commit_message>
I have done to create Register page,login page,home page and order page.
</commit_message>
<xml_diff>
--- a/Selenium_Main_Assignment/Resources/test_data.xlsx
+++ b/Selenium_Main_Assignment/Resources/test_data.xlsx
@@ -8,27 +8,99 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkunchala/pythonAssignments/Python_Assignments/Selenium_Main_Assignment/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9BAD4E-D4E8-0447-BDFB-15E89394124E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBE2784-C591-DE4A-B896-36F467C16820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Credit card</t>
+  </si>
+  <si>
+    <t>Raju</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Ongole</t>
+  </si>
+  <si>
+    <t>Nithish</t>
+  </si>
+  <si>
+    <t>Tamilnadu</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Raju123</t>
+  </si>
+  <si>
+    <t>Raju@123</t>
+  </si>
+  <si>
+    <t>Raju1</t>
+  </si>
+  <si>
+    <t>Raju@1234</t>
+  </si>
+  <si>
+    <t>Raju@12345</t>
+  </si>
+  <si>
+    <t>Rajuk</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF292B2C"/>
+      <name val="LatoWeb"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -51,13 +123,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -358,21 +436,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.83203125" customWidth="1"/>
     <col min="6" max="6" width="16.1640625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>123456789012345</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>123456789012945</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>2025</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B6A37B-6AC7-9943-A902-95773952D757}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A6E0378E-C8A3-6D47-B9BD-C77787FD25C4}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{1C554E58-A293-7040-AC8F-D86C6D18FB02}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{BF0E7F82-DD01-554F-801D-238EC7C2CD3A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I have done to create TakescreenShot page and write logger message and i have done few changes in code.
</commit_message>
<xml_diff>
--- a/Selenium_Main_Assignment/Resources/test_data.xlsx
+++ b/Selenium_Main_Assignment/Resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkunchala/pythonAssignments/Python_Assignments/Selenium_Main_Assignment/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBE2784-C591-DE4A-B896-36F467C16820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59466544-F150-B041-B0DC-8BEFB358D2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -78,13 +78,49 @@
   </si>
   <si>
     <t>Rajuk</t>
+  </si>
+  <si>
+    <t>Hashedin</t>
+  </si>
+  <si>
+    <t>Hashedin@123</t>
+  </si>
+  <si>
+    <t>Hashedin1</t>
+  </si>
+  <si>
+    <t>Hashedin@124</t>
+  </si>
+  <si>
+    <t>Hashedin2</t>
+  </si>
+  <si>
+    <t>Hashedin@125</t>
+  </si>
+  <si>
+    <t>Hashedin3</t>
+  </si>
+  <si>
+    <t>Hashedin@126</t>
+  </si>
+  <si>
+    <t>Hashedin4</t>
+  </si>
+  <si>
+    <t>Hashedin@127</t>
+  </si>
+  <si>
+    <t>Hashedin5</t>
+  </si>
+  <si>
+    <t>Hashedin@128</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +137,26 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF292B2C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF292B2C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,12 +183,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -438,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -518,10 +576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B6A37B-6AC7-9943-A902-95773952D757}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -530,44 +588,109 @@
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="20">
+      <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:3" ht="19">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{A6E0378E-C8A3-6D47-B9BD-C77787FD25C4}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{1C554E58-A293-7040-AC8F-D86C6D18FB02}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{BF0E7F82-DD01-554F-801D-238EC7C2CD3A}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{A6E0378E-C8A3-6D47-B9BD-C77787FD25C4}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{1C554E58-A293-7040-AC8F-D86C6D18FB02}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{BF0E7F82-DD01-554F-801D-238EC7C2CD3A}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{B3CC6856-DFBE-F244-B522-E8E1A28784F3}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{8C87A02D-8AC9-E242-958E-A359BFE6A608}"/>
+    <hyperlink ref="B7" r:id="rId6" display="Hashedin@123" xr:uid="{674243BF-725C-814C-8D17-47821CB6D8DF}"/>
+    <hyperlink ref="B8" r:id="rId7" display="Hashedin@123" xr:uid="{331FDEE7-6555-934A-9BDD-37A64D06DCD4}"/>
+    <hyperlink ref="B9" r:id="rId8" display="Hashedin@123" xr:uid="{E8B198C0-EEEE-954D-A641-A54D7FEBA567}"/>
+    <hyperlink ref="B10" r:id="rId9" display="Hashedin@123" xr:uid="{A5675A88-7C8A-5747-B287-FB8E1B7715EB}"/>
+    <hyperlink ref="B11" r:id="rId10" display="Hashedin@123" xr:uid="{198B46D1-6A71-7F4D-896B-2143A3A59AE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>